<commit_message>
So many corrections to ticket code
</commit_message>
<xml_diff>
--- a/test/fixtures/files/invalid_tickets.xlsx
+++ b/test/fixtures/files/invalid_tickets.xlsx
@@ -22,7 +22,7 @@
     <t>Time</t>
   </si>
   <si>
-    <t>First Name</t>
+    <t>Name</t>
   </si>
   <si>
     <t>Last Name</t>
@@ -40,13 +40,13 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>Booking Number</t>
-  </si>
-  <si>
-    <t>Ticket Number</t>
-  </si>
-  <si>
-    <t>Ticket Type</t>
+    <t>Booking#</t>
+  </si>
+  <si>
+    <t>Registration#</t>
+  </si>
+  <si>
+    <t>Registration Type</t>
   </si>
   <si>
     <t>Booking Type</t>
@@ -163,7 +163,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -195,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -208,6 +208,9 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -527,19 +530,19 @@
     <col min="2" max="2" style="5" width="10.719285714285713" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="5.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="7.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="7.433571428571429" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="5" width="15.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="10.290714285714287" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="5" width="14.862142857142858" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="5" width="24.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="17.719285714285714" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="5" width="25.576428571428572" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="5" width="10.290714285714287" customWidth="1" bestFit="1"/>
     <col min="14" max="14" style="5" width="10.290714285714287" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="5" width="10.290714285714287" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="5" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="6" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="7" width="10.290714285714287" customWidth="1" bestFit="1"/>
     <col min="18" max="18" style="5" width="10.290714285714287" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="5" width="10.290714285714287" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="5" width="17.005" customWidth="1" bestFit="1"/>
@@ -547,13 +550,13 @@
     <col min="22" max="22" style="5" width="11.290714285714287" customWidth="1" bestFit="1"/>
     <col min="23" max="23" style="5" width="11.147857142857141" customWidth="1" bestFit="1"/>
     <col min="24" max="24" style="5" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="5" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="6" width="11.290714285714287" customWidth="1" bestFit="1"/>
     <col min="26" max="26" style="5" width="11.290714285714287" customWidth="1" bestFit="1"/>
     <col min="27" max="27" style="5" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="5" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="6" width="11.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,7 +642,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Update to CrowdFlo import process
</commit_message>
<xml_diff>
--- a/test/fixtures/files/invalid_tickets.xlsx
+++ b/test/fixtures/files/invalid_tickets.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -52,52 +52,49 @@
     <t>Booking Type</t>
   </si>
   <si>
+    <t>Question 16</t>
+  </si>
+  <si>
+    <t>Question 6</t>
+  </si>
+  <si>
+    <t>Question 8</t>
+  </si>
+  <si>
+    <t>Question 15</t>
+  </si>
+  <si>
+    <t>Question 14</t>
+  </si>
+  <si>
+    <t>Question 3</t>
+  </si>
+  <si>
+    <t>Question 9</t>
+  </si>
+  <si>
     <t>Question 13</t>
   </si>
   <si>
-    <t>Question 9</t>
-  </si>
-  <si>
-    <t>Question 14</t>
+    <t>Question 2</t>
+  </si>
+  <si>
+    <t>Question 7</t>
+  </si>
+  <si>
+    <t>Question 4</t>
+  </si>
+  <si>
+    <t>Question 12</t>
+  </si>
+  <si>
+    <t>Question 10</t>
+  </si>
+  <si>
+    <t>Question 11</t>
   </si>
   <si>
     <t>Question 1</t>
-  </si>
-  <si>
-    <t>Question 8</t>
-  </si>
-  <si>
-    <t>Question 6</t>
-  </si>
-  <si>
-    <t>Question 15</t>
-  </si>
-  <si>
-    <t>Question 4</t>
-  </si>
-  <si>
-    <t>Question 12</t>
-  </si>
-  <si>
-    <t>Question 5</t>
-  </si>
-  <si>
-    <t>Question 7</t>
-  </si>
-  <si>
-    <t>Question 10</t>
-  </si>
-  <si>
-    <t>Question 2</t>
-  </si>
-  <si>
-    <t>Question 11</t>
-  </si>
-  <si>
-    <t>Question 3</t>
-  </si>
-  <si>
-    <t>Question 16</t>
   </si>
   <si>
     <t>2/06/2023</t>
@@ -556,7 +553,7 @@
     <col min="28" max="28" style="6" width="11.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,90 +630,90 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" s="4">
         <v>417858583</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="N2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="4">
         <v>23</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="V2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y2" s="3"/>
       <c r="Z2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="AB2" s="3"/>
     </row>

</xml_diff>